<commit_message>
fully work save load system with major server crash bug fixes
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7558C5AB-FB47-49DE-B167-02C7A6DC1F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D71BCA-7C2B-4739-B734-0A3DBC91948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>сделать спавн предметов для починки на каждом этаже в зависимости от типа выхода 100%</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Пофиксить краш сервера при попытки зайти с одинаковым ником</t>
+  </si>
+  <si>
+    <t>Cделано</t>
+  </si>
+  <si>
+    <t>В процессе</t>
+  </si>
+  <si>
+    <t>Добавить новый тип предметов (Документы)</t>
   </si>
 </sst>
 </file>
@@ -100,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +131,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -168,6 +189,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,16 +476,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -495,8 +523,11 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -519,8 +550,8 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -599,7 +630,15 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
client print word wrap fix (again blyat)
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D71BCA-7C2B-4739-B734-0A3DBC91948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7DCF10-9841-4C16-B9E9-8ECE294CECAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,8 +590,8 @@
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix add player item from enemy if inventory is full
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7DCF10-9841-4C16-B9E9-8ECE294CECAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD5DECE-39A3-4E55-81C3-BE8145244331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,8 +501,8 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
now elevator is broken at start, repair items 100% will be found on location, + generations fix
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD5DECE-39A3-4E55-81C3-BE8145244331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FECFEA-5475-4FAE-8B4A-55BB3EA26587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,8 +493,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
+      <c r="B1" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -512,8 +512,8 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>14</v>
@@ -622,8 +622,8 @@
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
+      <c r="B16" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
server notify new player
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FECFEA-5475-4FAE-8B4A-55BB3EA26587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25B198D-F9CD-4ACB-98B6-D83901BAB918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>сделать спавн предметов для починки на каждом этаже в зависимости от типа выхода 100%</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Добавить новый тип предметов (Документы)</t>
+  </si>
+  <si>
+    <t>Добавить оповещение о присоединении игрока</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,6 +645,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add player disconnect notify
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25B198D-F9CD-4ACB-98B6-D83901BAB918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4EE78B-E03B-4269-9E5A-E01FF86C3AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
     <t>Добавить новый тип предметов (Документы)</t>
   </si>
   <si>
-    <t>Добавить оповещение о присоединении игрока</t>
+    <t>Добавить оповещение о присоединении и выходе игрока</t>
   </si>
 </sst>
 </file>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add samosbor base system
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4EE78B-E03B-4269-9E5A-E01FF86C3AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9630252-2D79-4CE4-B50F-BA9578169AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>делать клиенту деструктор</t>
   </si>
   <si>
-    <t>добавить систему рецептов из одно рецепта</t>
-  </si>
-  <si>
     <t>добавить сохранения и загрузку(Бинарник)</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Добавить оповещение о присоединении и выходе игрока</t>
+  </si>
+  <si>
+    <t>добавить систему рецептов из одного рецепта</t>
   </si>
 </sst>
 </file>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -505,10 +505,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,10 +516,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,10 +527,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,119 +538,119 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully work samosbor system, + major bugfixes
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9630252-2D79-4CE4-B50F-BA9578169AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B91172-15C2-4551-96B7-2A5A8EC2E198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>сделать спавн предметов для починки на каждом этаже в зависимости от типа выхода 100%</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>добавить систему рецептов из одного рецепта</t>
+  </si>
+  <si>
+    <t>Добавить массив не тратящихся элементов в крафтах</t>
+  </si>
+  <si>
+    <t>Добавить стамину</t>
+  </si>
+  <si>
+    <t>0.6.0</t>
   </si>
 </sst>
 </file>
@@ -112,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +158,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -177,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -198,6 +213,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,12 +510,15 @@
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -507,6 +528,9 @@
       <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
@@ -518,6 +542,9 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C3" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
@@ -529,6 +556,9 @@
       <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C4" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
@@ -556,6 +586,9 @@
       <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -577,8 +610,11 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>20</v>
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -596,6 +632,9 @@
       <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C12" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -628,16 +667,22 @@
       <c r="B16" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -645,12 +690,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
load start samosbor fix
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B91172-15C2-4551-96B7-2A5A8EC2E198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC567F3C-221E-4E75-8269-D97ACF974C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
   <si>
     <t>сделать спавн предметов для починки на каждом этаже в зависимости от типа выхода 100%</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Добавить оповещение о присоединении и выходе игрока</t>
   </si>
   <si>
-    <t>добавить систему рецептов из одного рецепта</t>
-  </si>
-  <si>
     <t>Добавить массив не тратящихся элементов в крафтах</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>0.6.0</t>
+  </si>
+  <si>
+    <t>добавить систему рецептов из одного предмета и просмотр крафта определенного предмета</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
@@ -543,7 +543,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
@@ -557,7 +557,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>20</v>
@@ -571,12 +571,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,7 +590,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -602,8 +605,11 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,7 +620,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -633,7 +639,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -656,8 +662,11 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>7</v>
+      <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -668,7 +677,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -679,7 +688,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,12 +707,12 @@
         <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -711,7 +720,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
now you can attack with fists
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC567F3C-221E-4E75-8269-D97ACF974C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5282B440-D5EA-4164-8B79-C7219EFC88DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
   <si>
     <t>сделать спавн предметов для починки на каждом этаже в зависимости от типа выхода 100%</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>добавить систему рецептов из одного предмета и просмотр крафта определенного предмета</t>
+  </si>
+  <si>
+    <t>Сделать возможность бить руками</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,6 +729,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add say command, just chatting in game
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37226772-D3CC-4BD6-8120-851EDD67A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882F0EE1-C62D-43F6-A05C-F4801086234B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>сделать спавн предметов для починки на каждом этаже в зависимости от типа выхода 100%</t>
   </si>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,8 +651,8 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>25</v>
@@ -711,12 +711,10 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -804,12 +802,10 @@
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">

</xml_diff>

<commit_message>
add autosave for game
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882F0EE1-C62D-43F6-A05C-F4801086234B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73992BC1-C88B-4B3A-8996-36BE46390E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -238,9 +238,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -544,7 +541,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,13 +552,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -572,10 +569,10 @@
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -586,10 +583,10 @@
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -600,10 +597,10 @@
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -614,7 +611,7 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -623,7 +620,7 @@
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -634,7 +631,7 @@
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -645,7 +642,7 @@
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -654,7 +651,7 @@
       <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -665,7 +662,7 @@
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -676,7 +673,7 @@
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -685,7 +682,7 @@
       <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -696,7 +693,7 @@
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -705,7 +702,7 @@
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -714,7 +711,7 @@
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -723,7 +720,7 @@
       <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -734,7 +731,7 @@
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -745,7 +742,7 @@
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -754,7 +751,7 @@
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -765,7 +762,7 @@
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -774,7 +771,7 @@
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -783,7 +780,7 @@
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -791,10 +788,10 @@
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -805,7 +802,7 @@
       <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -814,7 +811,7 @@
       <c r="B25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix load game entity descriptions
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hejdj\Desktop\Крутой хакерман ыыы\GigahrushMUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73992BC1-C88B-4B3A-8996-36BE46390E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C78996-B469-4E0C-9014-B41E8127F90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>